<commit_message>
okok Signed-off-by: YooSeongHyun <wtnghw@naver.com>
</commit_message>
<xml_diff>
--- a/프로젝트/Ganttchart.xlsx
+++ b/프로젝트/Ganttchart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>요구분석 단계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,95 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9월 21일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9월 22일</t>
-  </si>
-  <si>
-    <t>9월 23일</t>
-  </si>
-  <si>
-    <t>9월 24일</t>
-  </si>
-  <si>
-    <t>9월 25일</t>
-  </si>
-  <si>
-    <t>9월 26일</t>
-  </si>
-  <si>
-    <t>9월 27일</t>
-  </si>
-  <si>
-    <t>9월 28일</t>
-  </si>
-  <si>
-    <t>9월 29일</t>
-  </si>
-  <si>
-    <t>9월 30일</t>
-  </si>
-  <si>
-    <t>10월 1일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10월 2일</t>
-  </si>
-  <si>
-    <t>10월 3일</t>
-  </si>
-  <si>
-    <t>10월 4일</t>
-  </si>
-  <si>
-    <t>10월 5일</t>
-  </si>
-  <si>
-    <t>10월 6일</t>
-  </si>
-  <si>
-    <t>10월 7일</t>
-  </si>
-  <si>
-    <t>10월 8일</t>
-  </si>
-  <si>
-    <t>10월 9일</t>
-  </si>
-  <si>
-    <t>10월 10일</t>
-  </si>
-  <si>
-    <t>10월 11일</t>
-  </si>
-  <si>
-    <t>10월 12일</t>
-  </si>
-  <si>
-    <t>10월 13일</t>
-  </si>
-  <si>
-    <t>10월 14일</t>
-  </si>
-  <si>
-    <t>10월 15일</t>
-  </si>
-  <si>
-    <t>10월 16일</t>
-  </si>
-  <si>
-    <t>10월 17일</t>
-  </si>
-  <si>
-    <t>10월 18일</t>
-  </si>
-  <si>
-    <t>10월 19일</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - 시스템설계서</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -151,6 +62,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="m&quot;/&quot;d;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,14 +82,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -187,6 +93,14 @@
     <font>
       <b/>
       <sz val="26"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -214,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -496,39 +410,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -550,28 +438,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1">
@@ -583,44 +462,44 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,14 +573,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>40822</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>457200</xdr:rowOff>
     </xdr:to>
@@ -712,8 +591,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4114800" y="2162175"/>
-          <a:ext cx="1323975" cy="400050"/>
+          <a:off x="2939143" y="2152650"/>
+          <a:ext cx="1258661" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -820,8 +699,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8915400" y="3190875"/>
-          <a:ext cx="1343025" cy="400050"/>
+          <a:off x="6410325" y="3186793"/>
+          <a:ext cx="842282" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -857,15 +736,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>457200</xdr:rowOff>
+      <xdr:rowOff>466725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -874,62 +753,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10286999" y="3705225"/>
-          <a:ext cx="9525001" cy="400050"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>466725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="오른쪽 화살표 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17145000" y="4229100"/>
-          <a:ext cx="4067175" cy="400050"/>
+          <a:off x="10315575" y="3714750"/>
+          <a:ext cx="7477125" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -965,13 +790,67 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="오른쪽 화살표 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17821275" y="4229100"/>
+          <a:ext cx="1333500" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>657224</xdr:colOff>
+      <xdr:colOff>657223</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>476250</xdr:rowOff>
     </xdr:to>
@@ -982,8 +861,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17830800" y="4752975"/>
-          <a:ext cx="3371849" cy="400050"/>
+          <a:off x="19202399" y="4752975"/>
+          <a:ext cx="2000249" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -1065,6 +944,273 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="모서리가 둥근 사각형 설명선 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4286250" y="1619250"/>
+          <a:ext cx="1592036" cy="557893"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -54166"/>
+            <a:gd name="adj2" fmla="val 84451"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>9/25</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>오전 리뷰</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>97972</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>220437</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>478971</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="모서리가 둥근 사각형 설명선 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13337722" y="4084864"/>
+          <a:ext cx="1592036" cy="557893"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -54166"/>
+            <a:gd name="adj2" fmla="val 84451"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>10/16</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>오후 리뷰</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>141516</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>299358</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>495300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="모서리가 둥근 사각형 설명선 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7394123" y="3265714"/>
+          <a:ext cx="1028699" cy="359229"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -54166"/>
+            <a:gd name="adj2" fmla="val 84451"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>10/3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 리뷰</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1360,15 +1506,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="21" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="31" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1402,11 +1553,11 @@
       <c r="AC1" s="21"/>
       <c r="AD1" s="21"/>
       <c r="AE1" s="21"/>
-      <c r="AF1" s="19"/>
+      <c r="AF1" s="15"/>
     </row>
     <row r="2" spans="2:32" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="22" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1439,93 +1590,93 @@
       <c r="AE2" s="24"/>
     </row>
     <row r="3" spans="2:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="U3" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W3" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="X3" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y3" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z3" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA3" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB3" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC3" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD3" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE3" s="30" t="s">
-        <v>34</v>
+      <c r="B3" s="16"/>
+      <c r="C3" s="25">
+        <v>42268</v>
+      </c>
+      <c r="D3" s="25">
+        <v>42269</v>
+      </c>
+      <c r="E3" s="25">
+        <v>42270</v>
+      </c>
+      <c r="F3" s="25">
+        <v>42271</v>
+      </c>
+      <c r="G3" s="25">
+        <v>42272</v>
+      </c>
+      <c r="H3" s="25">
+        <v>42273</v>
+      </c>
+      <c r="I3" s="25">
+        <v>42274</v>
+      </c>
+      <c r="J3" s="25">
+        <v>42275</v>
+      </c>
+      <c r="K3" s="25">
+        <v>42276</v>
+      </c>
+      <c r="L3" s="25">
+        <v>42277</v>
+      </c>
+      <c r="M3" s="25">
+        <v>42278</v>
+      </c>
+      <c r="N3" s="25">
+        <v>42279</v>
+      </c>
+      <c r="O3" s="25">
+        <v>42280</v>
+      </c>
+      <c r="P3" s="25">
+        <v>42281</v>
+      </c>
+      <c r="Q3" s="25">
+        <v>42282</v>
+      </c>
+      <c r="R3" s="25">
+        <v>42283</v>
+      </c>
+      <c r="S3" s="25">
+        <v>42284</v>
+      </c>
+      <c r="T3" s="25">
+        <v>42285</v>
+      </c>
+      <c r="U3" s="25">
+        <v>42286</v>
+      </c>
+      <c r="V3" s="25">
+        <v>42287</v>
+      </c>
+      <c r="W3" s="25">
+        <v>42288</v>
+      </c>
+      <c r="X3" s="25">
+        <v>42289</v>
+      </c>
+      <c r="Y3" s="25">
+        <v>42290</v>
+      </c>
+      <c r="Z3" s="25">
+        <v>42291</v>
+      </c>
+      <c r="AA3" s="25">
+        <v>42292</v>
+      </c>
+      <c r="AB3" s="25">
+        <v>42293</v>
+      </c>
+      <c r="AC3" s="25">
+        <v>42294</v>
+      </c>
+      <c r="AD3" s="25">
+        <v>42295</v>
+      </c>
+      <c r="AE3" s="25">
+        <v>42296</v>
       </c>
     </row>
     <row r="4" spans="2:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1538,33 +1689,33 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="25"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="1"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="25"/>
+      <c r="P4" s="17"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-      <c r="W4" s="25"/>
+      <c r="W4" s="17"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
-      <c r="AD4" s="25"/>
+      <c r="AD4" s="17"/>
       <c r="AE4" s="8"/>
     </row>
     <row r="5" spans="2:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>35</v>
+      <c r="B5" s="26" t="s">
+        <v>6</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
@@ -1572,29 +1723,29 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="26"/>
+      <c r="I5" s="18"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="26"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
-      <c r="W5" s="26"/>
+      <c r="W5" s="18"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="10"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="9"/>
     </row>
     <row r="6" spans="2:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
@@ -1606,33 +1757,33 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="27"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="3"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="27"/>
+      <c r="P6" s="19"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
-      <c r="W6" s="27"/>
+      <c r="W6" s="19"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
-      <c r="AD6" s="27"/>
-      <c r="AE6" s="11"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="10"/>
     </row>
     <row r="7" spans="2:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
-        <v>35</v>
+      <c r="B7" s="27" t="s">
+        <v>6</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
@@ -1640,33 +1791,33 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="26"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
-      <c r="P7" s="26"/>
+      <c r="P7" s="18"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
-      <c r="W7" s="26"/>
+      <c r="W7" s="18"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
-      <c r="AD7" s="26"/>
-      <c r="AE7" s="10"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="9"/>
     </row>
     <row r="8" spans="2:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
-        <v>36</v>
+      <c r="B8" s="27" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="6"/>
@@ -1674,33 +1825,33 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="27"/>
+      <c r="I8" s="19"/>
       <c r="J8" s="3"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="27"/>
+      <c r="P8" s="19"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
-      <c r="W8" s="27"/>
+      <c r="W8" s="19"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
-      <c r="AD8" s="27"/>
-      <c r="AE8" s="11"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="10"/>
     </row>
     <row r="9" spans="2:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
-        <v>37</v>
+      <c r="B9" s="26" t="s">
+        <v>8</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
@@ -1708,29 +1859,29 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="26"/>
+      <c r="I9" s="18"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
-      <c r="P9" s="26"/>
+      <c r="P9" s="18"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
-      <c r="W9" s="26"/>
+      <c r="W9" s="18"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="10"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="9"/>
     </row>
     <row r="10" spans="2:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
@@ -1742,29 +1893,29 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="27"/>
+      <c r="I10" s="19"/>
       <c r="J10" s="3"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="27"/>
+      <c r="P10" s="19"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
-      <c r="W10" s="27"/>
+      <c r="W10" s="19"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
-      <c r="AD10" s="27"/>
-      <c r="AE10" s="11"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="10"/>
     </row>
     <row r="11" spans="2:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
@@ -1776,29 +1927,29 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="26"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="26"/>
+      <c r="P11" s="18"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
-      <c r="W11" s="26"/>
+      <c r="W11" s="18"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
-      <c r="AD11" s="26"/>
-      <c r="AE11" s="10"/>
+      <c r="AD11" s="18"/>
+      <c r="AE11" s="9"/>
     </row>
     <row r="12" spans="2:32" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
@@ -1810,63 +1961,63 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="26"/>
+      <c r="I12" s="18"/>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
-      <c r="P12" s="26"/>
+      <c r="P12" s="18"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
-      <c r="W12" s="26"/>
+      <c r="W12" s="18"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
-      <c r="AD12" s="26"/>
-      <c r="AE12" s="10"/>
+      <c r="AD12" s="18"/>
+      <c r="AE12" s="9"/>
     </row>
     <row r="13" spans="2:32" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="16"/>
-      <c r="AD13" s="28"/>
-      <c r="AE13" s="17"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
+      <c r="AC13" s="13"/>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1875,7 +2026,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>